<commit_message>
Small bugs and adjstments
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_FT_2023/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA3893E-975E-C34B-85CB-F895FE3E794E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F609BC5A-B230-5647-A512-E092BA3D2B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="224">
   <si>
     <t>Source</t>
   </si>
@@ -703,13 +703,16 @@
     <t>For SA cases only 5 points</t>
   </si>
   <si>
-    <t>Days FT prod. For sto max cap.</t>
-  </si>
-  <si>
     <t>Max elec. Price</t>
   </si>
   <si>
     <t>Standard set for STP at max 14 days worth of FT hyd. Consumpt.</t>
+  </si>
+  <si>
+    <t>Days FT prod. for sto max cap.</t>
+  </si>
+  <si>
+    <t>Cooper</t>
   </si>
 </sst>
 </file>
@@ -3517,12 +3520,12 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -3713,10 +3716,10 @@
         <v>99</v>
       </c>
       <c r="I19" t="s">
+        <v>222</v>
+      </c>
+      <c r="J19" t="s">
         <v>220</v>
-      </c>
-      <c r="J19" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -3747,11 +3750,11 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H23" si="0">ABS(E20)*24*I20</f>
+        <f>ABS(E20)*24*I20</f>
         <v>1188267.024</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:I22" si="1">ROUNDUP(J20*$I$24/$J$24,0)</f>
+        <f t="shared" ref="I20:I22" si="0">ROUNDUP(J20*$I$24/$J$24,0)</f>
         <v>2</v>
       </c>
       <c r="J20">
@@ -3760,25 +3763,25 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="B21">
         <v>769</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:C24" si="2">MAX(-B21+$B$15, -1000+$B$15)</f>
+        <f t="shared" ref="C21:C24" si="1">MAX(-B21+$B$15, -1000+$B$15)</f>
         <v>-754.1</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D24" si="3">-100+$B$15</f>
+        <f t="shared" ref="D21:D24" si="2">-100+$B$15</f>
         <v>-85.1</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21" si="4">C21*25.13</f>
+        <f t="shared" ref="E21" si="3">C21*25.13</f>
         <v>-18950.532999999999</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21" si="5">D21*25.13</f>
+        <f t="shared" ref="F21" si="4">D21*25.13</f>
         <v>-2138.5629999999996</v>
       </c>
       <c r="G21">
@@ -3786,11 +3789,11 @@
         <v>0</v>
       </c>
       <c r="H21">
+        <f t="shared" ref="H20:H23" si="5">ABS(E21)*24*I21</f>
+        <v>3183689.5440000002</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="0"/>
-        <v>3183689.5440000002</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J21">
@@ -3805,11 +3808,11 @@
         <v>894</v>
       </c>
       <c r="C22">
+        <f t="shared" si="1"/>
+        <v>-879.1</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="2"/>
-        <v>-879.1</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
         <v>-85.1</v>
       </c>
       <c r="E22">
@@ -3825,11 +3828,11 @@
         <v>0</v>
       </c>
       <c r="H22">
+        <f t="shared" si="5"/>
+        <v>1060405.584</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="0"/>
-        <v>1060405.584</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J22">
@@ -3844,11 +3847,11 @@
         <v>522</v>
       </c>
       <c r="C23">
+        <f t="shared" si="1"/>
+        <v>-507.1</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="2"/>
-        <v>-507.1</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
         <v>-85.1</v>
       </c>
       <c r="E23">
@@ -3864,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>305842.152</v>
       </c>
       <c r="I23">
@@ -3883,11 +3886,11 @@
         <v>1280</v>
       </c>
       <c r="C24">
+        <f t="shared" si="1"/>
+        <v>-985.1</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="2"/>
-        <v>-985.1</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="3"/>
         <v>-85.1</v>
       </c>
       <c r="E24">
@@ -3913,7 +3916,7 @@
         <v>8997</v>
       </c>
       <c r="K24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -4495,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="32">
-        <f t="shared" ref="C44:K44" si="12">C$43*ABS($G20-$H20)/9</f>
+        <f t="shared" ref="C44:J44" si="12">C$43*ABS($G20-$H20)/9</f>
         <v>132029.66933333332</v>
       </c>
       <c r="D44" s="34">

</xml_diff>

<commit_message>
update inputs 0% initial storage and update sweep storage values, only up to 24h storage of ft capacity
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_FT_2023/data/HERON_data.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F609BC5A-B230-5647-A512-E092BA3D2B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B3E8E-5E1C-4B43-9BA0-77827BC645D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="7" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="Transfer_rates" sheetId="4" r:id="rId2"/>
     <sheet name="HTSE" sheetId="2" r:id="rId3"/>
     <sheet name="FT" sheetId="11" r:id="rId4"/>
-    <sheet name="Sweep values" sheetId="10" r:id="rId5"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
-    <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
+    <sheet name="sweep_values_storage" sheetId="15" r:id="rId5"/>
+    <sheet name="sweep_values_ft" sheetId="14" r:id="rId6"/>
+    <sheet name="sweep_values_htse" sheetId="13" r:id="rId7"/>
+    <sheet name="Sweep values" sheetId="10" r:id="rId8"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId9"/>
+    <sheet name="NPP_capacities" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="230">
   <si>
     <t>Source</t>
   </si>
@@ -713,6 +716,24 @@
   </si>
   <si>
     <t>Cooper</t>
+  </si>
+  <si>
+    <t>braidwood</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>davis_besse</t>
+  </si>
+  <si>
+    <t>prairie_island</t>
+  </si>
+  <si>
+    <t>stp</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -2565,11 +2586,315 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3645</v>
+      </c>
+      <c r="F2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="23">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J2" s="19">
+        <f>$B$10+I2*(1-$B$10)</f>
+        <v>0.28505000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2817</v>
+      </c>
+      <c r="F3">
+        <v>894</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19">
+        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3853</v>
+      </c>
+      <c r="F4">
+        <v>1280</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0</v>
+      </c>
+      <c r="J4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3411</v>
+      </c>
+      <c r="F5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" s="23">
+        <v>8.8400000000000006E-2</v>
+      </c>
+      <c r="J5" s="19">
+        <f t="shared" si="0"/>
+        <v>0.27983599999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1677</v>
+      </c>
+      <c r="F6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.28742000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2419</v>
+      </c>
+      <c r="F7">
+        <v>769</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I7" s="23">
+        <v>7.8100000000000003E-2</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.27169900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3990</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" s="23">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.24870999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="22">
+        <v>0.21</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="18"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3516,11 +3841,846 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C390E3C-C04B-274E-8588-FEE720CE7A6B}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>sweep_values_htse!A2</f>
+        <v>braidwood</v>
+      </c>
+      <c r="B2" s="32">
+        <f>'Sweep values'!B44</f>
+        <v>10</v>
+      </c>
+      <c r="C2" s="32">
+        <f>'Sweep values'!C44</f>
+        <v>66014.834666666662</v>
+      </c>
+      <c r="D2" s="32">
+        <f>'Sweep values'!D44</f>
+        <v>132029.66933333332</v>
+      </c>
+      <c r="E2" s="32">
+        <f>'Sweep values'!E44</f>
+        <v>198044.50399999999</v>
+      </c>
+      <c r="F2" s="32">
+        <f>'Sweep values'!F44</f>
+        <v>264059.33866666665</v>
+      </c>
+      <c r="G2" s="32">
+        <f>'Sweep values'!G44</f>
+        <v>330074.17333333334</v>
+      </c>
+      <c r="H2" s="32">
+        <f>'Sweep values'!H44</f>
+        <v>396089.00799999997</v>
+      </c>
+      <c r="I2" s="32">
+        <f>'Sweep values'!I44</f>
+        <v>462103.84266666666</v>
+      </c>
+      <c r="J2" s="32">
+        <f>'Sweep values'!J44</f>
+        <v>528118.6773333333</v>
+      </c>
+      <c r="K2" s="32">
+        <f>'Sweep values'!K44</f>
+        <v>594133.51199999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>sweep_values_htse!A3</f>
+        <v>cooper</v>
+      </c>
+      <c r="B3" s="32">
+        <f>'Sweep values'!B45</f>
+        <v>10</v>
+      </c>
+      <c r="C3" s="32">
+        <f>'Sweep values'!C45</f>
+        <v>50534.754666666668</v>
+      </c>
+      <c r="D3" s="32">
+        <f>'Sweep values'!D45</f>
+        <v>101069.50933333334</v>
+      </c>
+      <c r="E3" s="32">
+        <f>'Sweep values'!E45</f>
+        <v>151604.26400000002</v>
+      </c>
+      <c r="F3" s="32">
+        <f>'Sweep values'!F45</f>
+        <v>202139.01866666667</v>
+      </c>
+      <c r="G3" s="32">
+        <f>'Sweep values'!G45</f>
+        <v>252673.77333333332</v>
+      </c>
+      <c r="H3" s="32">
+        <f>'Sweep values'!H45</f>
+        <v>303208.52800000005</v>
+      </c>
+      <c r="I3" s="32">
+        <f>'Sweep values'!I45</f>
+        <v>353743.28266666667</v>
+      </c>
+      <c r="J3" s="32">
+        <f>'Sweep values'!J45</f>
+        <v>404278.03733333334</v>
+      </c>
+      <c r="K3" s="32">
+        <f>'Sweep values'!K45</f>
+        <v>454812.79200000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>sweep_values_htse!A4</f>
+        <v>davis_besse</v>
+      </c>
+      <c r="B4" s="32">
+        <f>'Sweep values'!B46</f>
+        <v>10</v>
+      </c>
+      <c r="C4" s="32">
+        <f>'Sweep values'!C46</f>
+        <v>58911.421333333332</v>
+      </c>
+      <c r="D4" s="32">
+        <f>'Sweep values'!D46</f>
+        <v>117822.84266666666</v>
+      </c>
+      <c r="E4" s="32">
+        <f>'Sweep values'!E46</f>
+        <v>176734.26400000002</v>
+      </c>
+      <c r="F4" s="32">
+        <f>'Sweep values'!F46</f>
+        <v>235645.68533333333</v>
+      </c>
+      <c r="G4" s="32">
+        <f>'Sweep values'!G46</f>
+        <v>294557.10666666669</v>
+      </c>
+      <c r="H4" s="32">
+        <f>'Sweep values'!H46</f>
+        <v>353468.52800000005</v>
+      </c>
+      <c r="I4" s="32">
+        <f>'Sweep values'!I46</f>
+        <v>412379.94933333335</v>
+      </c>
+      <c r="J4" s="32">
+        <f>'Sweep values'!J46</f>
+        <v>471291.37066666665</v>
+      </c>
+      <c r="K4" s="32">
+        <f>'Sweep values'!K46</f>
+        <v>530202.79200000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>sweep_values_htse!A5</f>
+        <v>prairie_island</v>
+      </c>
+      <c r="B5" s="32">
+        <f>'Sweep values'!B47</f>
+        <v>10</v>
+      </c>
+      <c r="C5" s="32">
+        <f>'Sweep values'!C47</f>
+        <v>33982.461333333333</v>
+      </c>
+      <c r="D5" s="32">
+        <f>'Sweep values'!D47</f>
+        <v>67964.922666666665</v>
+      </c>
+      <c r="E5" s="32">
+        <f>'Sweep values'!E47</f>
+        <v>101947.38400000001</v>
+      </c>
+      <c r="F5" s="32">
+        <f>'Sweep values'!F47</f>
+        <v>135929.84533333333</v>
+      </c>
+      <c r="G5" s="32">
+        <f>'Sweep values'!G47</f>
+        <v>169912.30666666667</v>
+      </c>
+      <c r="H5" s="32">
+        <f>'Sweep values'!H47</f>
+        <v>203894.76800000001</v>
+      </c>
+      <c r="I5" s="32">
+        <f>'Sweep values'!I47</f>
+        <v>237877.22933333335</v>
+      </c>
+      <c r="J5" s="32">
+        <f>'Sweep values'!J47</f>
+        <v>271859.69066666666</v>
+      </c>
+      <c r="K5" s="32">
+        <f>'Sweep values'!K47</f>
+        <v>305842.152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>sweep_values_htse!A6</f>
+        <v>stp</v>
+      </c>
+      <c r="B6" s="32">
+        <f>'Sweep values'!B48</f>
+        <v>10</v>
+      </c>
+      <c r="C6" s="32">
+        <f>'Sweep values'!C48</f>
+        <v>66014.834666666662</v>
+      </c>
+      <c r="D6" s="32">
+        <f>'Sweep values'!D48</f>
+        <v>132029.66933333332</v>
+      </c>
+      <c r="E6" s="32">
+        <f>'Sweep values'!E48</f>
+        <v>198044.50399999999</v>
+      </c>
+      <c r="F6" s="32">
+        <f>'Sweep values'!F48</f>
+        <v>264059.33866666665</v>
+      </c>
+      <c r="G6" s="32">
+        <f>'Sweep values'!G48</f>
+        <v>330074.17333333334</v>
+      </c>
+      <c r="H6" s="32">
+        <f>'Sweep values'!H48</f>
+        <v>396089.00799999997</v>
+      </c>
+      <c r="I6" s="32">
+        <f>'Sweep values'!I48</f>
+        <v>462103.84266666666</v>
+      </c>
+      <c r="J6" s="32">
+        <f>'Sweep values'!J48</f>
+        <v>528118.6773333333</v>
+      </c>
+      <c r="K6" s="32">
+        <f>'Sweep values'!K48</f>
+        <v>594133.51199999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FF8260-2E28-CC46-B717-134719FB1D76}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>sweep_values_htse!A2</f>
+        <v>braidwood</v>
+      </c>
+      <c r="B2" s="32">
+        <f>'Sweep values'!B36</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="C2" s="32">
+        <f>'Sweep values'!C36</f>
+        <v>-22242.562999999998</v>
+      </c>
+      <c r="D2" s="32">
+        <f>'Sweep values'!D36</f>
+        <v>-19729.562999999998</v>
+      </c>
+      <c r="E2" s="32">
+        <f>'Sweep values'!E36</f>
+        <v>-17216.562999999998</v>
+      </c>
+      <c r="F2" s="32">
+        <f>'Sweep values'!F36</f>
+        <v>-14703.562999999998</v>
+      </c>
+      <c r="G2" s="32">
+        <f>'Sweep values'!G36</f>
+        <v>-12190.562999999998</v>
+      </c>
+      <c r="H2" s="32">
+        <f>'Sweep values'!H36</f>
+        <v>-9677.5629999999983</v>
+      </c>
+      <c r="I2" s="32">
+        <f>'Sweep values'!I36</f>
+        <v>-7164.5629999999983</v>
+      </c>
+      <c r="J2" s="32">
+        <f>'Sweep values'!J36</f>
+        <v>-4651.5629999999983</v>
+      </c>
+      <c r="K2" s="32">
+        <f>'Sweep values'!K36</f>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>sweep_values_htse!A3</f>
+        <v>cooper</v>
+      </c>
+      <c r="B3" s="32">
+        <f>'Sweep values'!B37</f>
+        <v>-18950.532999999999</v>
+      </c>
+      <c r="C3" s="32">
+        <f>'Sweep values'!C37</f>
+        <v>-17082.536333333333</v>
+      </c>
+      <c r="D3" s="32">
+        <f>'Sweep values'!D37</f>
+        <v>-15214.539666666666</v>
+      </c>
+      <c r="E3" s="32">
+        <f>'Sweep values'!E37</f>
+        <v>-13346.542999999998</v>
+      </c>
+      <c r="F3" s="32">
+        <f>'Sweep values'!F37</f>
+        <v>-11478.546333333332</v>
+      </c>
+      <c r="G3" s="32">
+        <f>'Sweep values'!G37</f>
+        <v>-9610.5496666666659</v>
+      </c>
+      <c r="H3" s="32">
+        <f>'Sweep values'!H37</f>
+        <v>-7742.5529999999981</v>
+      </c>
+      <c r="I3" s="32">
+        <f>'Sweep values'!I37</f>
+        <v>-5874.5563333333321</v>
+      </c>
+      <c r="J3" s="32">
+        <f>'Sweep values'!J37</f>
+        <v>-4006.5596666666643</v>
+      </c>
+      <c r="K3" s="32">
+        <f>'Sweep values'!K37</f>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>sweep_values_htse!A4</f>
+        <v>davis_besse</v>
+      </c>
+      <c r="B4" s="32">
+        <f>'Sweep values'!B38</f>
+        <v>-22091.782999999999</v>
+      </c>
+      <c r="C4" s="32">
+        <f>'Sweep values'!C38</f>
+        <v>-19874.758555555556</v>
+      </c>
+      <c r="D4" s="32">
+        <f>'Sweep values'!D38</f>
+        <v>-17657.734111111109</v>
+      </c>
+      <c r="E4" s="32">
+        <f>'Sweep values'!E38</f>
+        <v>-15440.709666666666</v>
+      </c>
+      <c r="F4" s="32">
+        <f>'Sweep values'!F38</f>
+        <v>-13223.685222222221</v>
+      </c>
+      <c r="G4" s="32">
+        <f>'Sweep values'!G38</f>
+        <v>-11006.660777777777</v>
+      </c>
+      <c r="H4" s="32">
+        <f>'Sweep values'!H38</f>
+        <v>-8789.636333333332</v>
+      </c>
+      <c r="I4" s="32">
+        <f>'Sweep values'!I38</f>
+        <v>-6572.6118888888868</v>
+      </c>
+      <c r="J4" s="32">
+        <f>'Sweep values'!J38</f>
+        <v>-4355.5874444444416</v>
+      </c>
+      <c r="K4" s="32">
+        <f>'Sweep values'!K38</f>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>sweep_values_htse!A5</f>
+        <v>prairie_island</v>
+      </c>
+      <c r="B5" s="32">
+        <f>'Sweep values'!B39</f>
+        <v>-12743.423000000001</v>
+      </c>
+      <c r="C5" s="32">
+        <f>'Sweep values'!C39</f>
+        <v>-11565.105222222222</v>
+      </c>
+      <c r="D5" s="32">
+        <f>'Sweep values'!D39</f>
+        <v>-10386.787444444446</v>
+      </c>
+      <c r="E5" s="32">
+        <f>'Sweep values'!E39</f>
+        <v>-9208.4696666666678</v>
+      </c>
+      <c r="F5" s="32">
+        <f>'Sweep values'!F39</f>
+        <v>-8030.1518888888895</v>
+      </c>
+      <c r="G5" s="32">
+        <f>'Sweep values'!G39</f>
+        <v>-6851.8341111111113</v>
+      </c>
+      <c r="H5" s="32">
+        <f>'Sweep values'!H39</f>
+        <v>-5673.5163333333339</v>
+      </c>
+      <c r="I5" s="32">
+        <f>'Sweep values'!I39</f>
+        <v>-4495.1985555555566</v>
+      </c>
+      <c r="J5" s="32">
+        <f>'Sweep values'!J39</f>
+        <v>-3316.8807777777783</v>
+      </c>
+      <c r="K5" s="32">
+        <f>'Sweep values'!K39</f>
+        <v>-2138.5630000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>sweep_values_htse!A6</f>
+        <v>stp</v>
+      </c>
+      <c r="B6" s="32">
+        <f>'Sweep values'!B40</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="C6" s="32">
+        <f>'Sweep values'!C40</f>
+        <v>-22242.562999999998</v>
+      </c>
+      <c r="D6" s="32">
+        <f>'Sweep values'!D40</f>
+        <v>-19729.562999999998</v>
+      </c>
+      <c r="E6" s="32">
+        <f>'Sweep values'!E40</f>
+        <v>-17216.562999999998</v>
+      </c>
+      <c r="F6" s="32">
+        <f>'Sweep values'!F40</f>
+        <v>-14703.562999999998</v>
+      </c>
+      <c r="G6" s="32">
+        <f>'Sweep values'!G40</f>
+        <v>-12190.562999999998</v>
+      </c>
+      <c r="H6" s="32">
+        <f>'Sweep values'!H40</f>
+        <v>-9677.5629999999983</v>
+      </c>
+      <c r="I6" s="32">
+        <f>'Sweep values'!I40</f>
+        <v>-7164.5629999999983</v>
+      </c>
+      <c r="J6" s="32">
+        <f>'Sweep values'!J40</f>
+        <v>-4651.5629999999983</v>
+      </c>
+      <c r="K6" s="32">
+        <f>'Sweep values'!K40</f>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE0E8A7-1174-AD42-ADFA-AE70859F756F}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="32">
+        <f>'Sweep values'!B28</f>
+        <v>-985.1</v>
+      </c>
+      <c r="C2" s="32">
+        <f>'Sweep values'!C28</f>
+        <v>-885.1</v>
+      </c>
+      <c r="D2" s="32">
+        <f>'Sweep values'!D28</f>
+        <v>-785.1</v>
+      </c>
+      <c r="E2" s="32">
+        <f>'Sweep values'!E28</f>
+        <v>-685.1</v>
+      </c>
+      <c r="F2" s="32">
+        <f>'Sweep values'!F28</f>
+        <v>-585.1</v>
+      </c>
+      <c r="G2" s="32">
+        <f>'Sweep values'!G28</f>
+        <v>-485.1</v>
+      </c>
+      <c r="H2" s="32">
+        <f>'Sweep values'!H28</f>
+        <v>-385.1</v>
+      </c>
+      <c r="I2" s="32">
+        <f>'Sweep values'!I28</f>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="J2" s="32">
+        <f>'Sweep values'!J28</f>
+        <v>-185.10000000000002</v>
+      </c>
+      <c r="K2" s="32">
+        <f>'Sweep values'!K28</f>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="32">
+        <f>'Sweep values'!B29</f>
+        <v>-754.1</v>
+      </c>
+      <c r="C3" s="32">
+        <f>'Sweep values'!C29</f>
+        <v>-679.76666666666665</v>
+      </c>
+      <c r="D3" s="32">
+        <f>'Sweep values'!D29</f>
+        <v>-605.43333333333339</v>
+      </c>
+      <c r="E3" s="32">
+        <f>'Sweep values'!E29</f>
+        <v>-531.1</v>
+      </c>
+      <c r="F3" s="32">
+        <f>'Sweep values'!F29</f>
+        <v>-456.76666666666671</v>
+      </c>
+      <c r="G3" s="32">
+        <f>'Sweep values'!G29</f>
+        <v>-382.43333333333334</v>
+      </c>
+      <c r="H3" s="32">
+        <f>'Sweep values'!H29</f>
+        <v>-308.10000000000002</v>
+      </c>
+      <c r="I3" s="32">
+        <f>'Sweep values'!I29</f>
+        <v>-233.76666666666665</v>
+      </c>
+      <c r="J3" s="32">
+        <f>'Sweep values'!J29</f>
+        <v>-159.43333333333339</v>
+      </c>
+      <c r="K3" s="32">
+        <f>'Sweep values'!K29</f>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="32">
+        <f>'Sweep values'!B30</f>
+        <v>-879.1</v>
+      </c>
+      <c r="C4" s="32">
+        <f>'Sweep values'!C30</f>
+        <v>-790.87777777777774</v>
+      </c>
+      <c r="D4" s="32">
+        <f>'Sweep values'!D30</f>
+        <v>-702.65555555555557</v>
+      </c>
+      <c r="E4" s="32">
+        <f>'Sweep values'!E30</f>
+        <v>-614.43333333333339</v>
+      </c>
+      <c r="F4" s="32">
+        <f>'Sweep values'!F30</f>
+        <v>-526.21111111111111</v>
+      </c>
+      <c r="G4" s="32">
+        <f>'Sweep values'!G30</f>
+        <v>-437.98888888888894</v>
+      </c>
+      <c r="H4" s="32">
+        <f>'Sweep values'!H30</f>
+        <v>-349.76666666666665</v>
+      </c>
+      <c r="I4" s="32">
+        <f>'Sweep values'!I30</f>
+        <v>-261.54444444444448</v>
+      </c>
+      <c r="J4" s="32">
+        <f>'Sweep values'!J30</f>
+        <v>-173.32222222222219</v>
+      </c>
+      <c r="K4" s="32">
+        <f>'Sweep values'!K30</f>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="32">
+        <f>'Sweep values'!B31</f>
+        <v>-507.1</v>
+      </c>
+      <c r="C5" s="32">
+        <f>'Sweep values'!C31</f>
+        <v>-460.21111111111111</v>
+      </c>
+      <c r="D5" s="32">
+        <f>'Sweep values'!D31</f>
+        <v>-413.32222222222225</v>
+      </c>
+      <c r="E5" s="32">
+        <f>'Sweep values'!E31</f>
+        <v>-366.43333333333339</v>
+      </c>
+      <c r="F5" s="32">
+        <f>'Sweep values'!F31</f>
+        <v>-319.54444444444448</v>
+      </c>
+      <c r="G5" s="32">
+        <f>'Sweep values'!G31</f>
+        <v>-272.65555555555557</v>
+      </c>
+      <c r="H5" s="32">
+        <f>'Sweep values'!H31</f>
+        <v>-225.76666666666671</v>
+      </c>
+      <c r="I5" s="32">
+        <f>'Sweep values'!I31</f>
+        <v>-178.87777777777779</v>
+      </c>
+      <c r="J5" s="32">
+        <f>'Sweep values'!J31</f>
+        <v>-131.98888888888894</v>
+      </c>
+      <c r="K5" s="32">
+        <f>'Sweep values'!K31</f>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="32">
+        <f>'Sweep values'!B32</f>
+        <v>-985.1</v>
+      </c>
+      <c r="C6" s="32">
+        <f>'Sweep values'!C32</f>
+        <v>-885.1</v>
+      </c>
+      <c r="D6" s="32">
+        <f>'Sweep values'!D32</f>
+        <v>-785.1</v>
+      </c>
+      <c r="E6" s="32">
+        <f>'Sweep values'!E32</f>
+        <v>-685.1</v>
+      </c>
+      <c r="F6" s="32">
+        <f>'Sweep values'!F32</f>
+        <v>-585.1</v>
+      </c>
+      <c r="G6" s="32">
+        <f>'Sweep values'!G32</f>
+        <v>-485.1</v>
+      </c>
+      <c r="H6" s="32">
+        <f>'Sweep values'!H32</f>
+        <v>-385.1</v>
+      </c>
+      <c r="I6" s="32">
+        <f>'Sweep values'!I32</f>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="J6" s="32">
+        <f>'Sweep values'!J32</f>
+        <v>-185.10000000000002</v>
+      </c>
+      <c r="K6" s="32">
+        <f>'Sweep values'!K32</f>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3750,8 +4910,8 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f>ABS(E20)*24*I20</f>
-        <v>1188267.024</v>
+        <f>ABS(E20)*24</f>
+        <v>594133.51199999999</v>
       </c>
       <c r="I20">
         <f t="shared" ref="I20:I22" si="0">ROUNDUP(J20*$I$24/$J$24,0)</f>
@@ -3789,8 +4949,8 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H20:H23" si="5">ABS(E21)*24*I21</f>
-        <v>3183689.5440000002</v>
+        <f t="shared" ref="H21:H24" si="5">ABS(E21)*24</f>
+        <v>454812.79200000002</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
@@ -3829,7 +4989,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="5"/>
-        <v>1060405.584</v>
+        <v>530202.79200000002</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
@@ -3906,8 +5066,8 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <f>ABS(E24)*24*I24</f>
-        <v>8317869.1679999996</v>
+        <f t="shared" si="5"/>
+        <v>594133.51199999999</v>
       </c>
       <c r="I24">
         <v>14</v>
@@ -4494,44 +5654,43 @@
         <v>143</v>
       </c>
       <c r="B44" s="34">
-        <f>B$43*ABS($G20-$H20)/9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C44" s="32">
-        <f t="shared" ref="C44:J44" si="12">C$43*ABS($G20-$H20)/9</f>
+        <f>C$43*ABS($G20-$H20)/9</f>
+        <v>66014.834666666662</v>
+      </c>
+      <c r="D44" s="34">
+        <f t="shared" ref="C44:J44" si="12">D$43*ABS($G20-$H20)/9</f>
         <v>132029.66933333332</v>
       </c>
-      <c r="D44" s="34">
+      <c r="E44" s="32">
+        <f t="shared" si="12"/>
+        <v>198044.50399999999</v>
+      </c>
+      <c r="F44" s="34">
         <f t="shared" si="12"/>
         <v>264059.33866666665</v>
       </c>
-      <c r="E44" s="32">
+      <c r="G44" s="32">
+        <f t="shared" si="12"/>
+        <v>330074.17333333334</v>
+      </c>
+      <c r="H44" s="34">
         <f t="shared" si="12"/>
         <v>396089.00799999997</v>
       </c>
-      <c r="F44" s="34">
+      <c r="I44" s="32">
+        <f t="shared" si="12"/>
+        <v>462103.84266666666</v>
+      </c>
+      <c r="J44" s="34">
         <f t="shared" si="12"/>
         <v>528118.6773333333</v>
       </c>
-      <c r="G44" s="32">
-        <f t="shared" si="12"/>
-        <v>660148.34666666668</v>
-      </c>
-      <c r="H44" s="34">
-        <f t="shared" si="12"/>
-        <v>792178.01599999995</v>
-      </c>
-      <c r="I44" s="32">
-        <f t="shared" si="12"/>
-        <v>924207.68533333333</v>
-      </c>
-      <c r="J44" s="34">
-        <f t="shared" si="12"/>
-        <v>1056237.3546666666</v>
-      </c>
       <c r="K44" s="32">
         <f>K$43*ABS($G20-$H20)/9</f>
-        <v>1188267.024</v>
+        <v>594133.51199999999</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -4539,44 +5698,43 @@
         <v>163</v>
       </c>
       <c r="B45" s="34">
-        <f t="shared" ref="B45:K45" si="13">B$43*ABS($G21-$H21)/9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C45" s="32">
+        <f t="shared" ref="B45:K45" si="13">C$43*ABS($G21-$H21)/9</f>
+        <v>50534.754666666668</v>
+      </c>
+      <c r="D45" s="34">
+        <f t="shared" si="13"/>
+        <v>101069.50933333334</v>
+      </c>
+      <c r="E45" s="32">
+        <f t="shared" si="13"/>
+        <v>151604.26400000002</v>
+      </c>
+      <c r="F45" s="34">
+        <f t="shared" si="13"/>
+        <v>202139.01866666667</v>
+      </c>
+      <c r="G45" s="32">
+        <f t="shared" si="13"/>
+        <v>252673.77333333332</v>
+      </c>
+      <c r="H45" s="34">
+        <f t="shared" si="13"/>
+        <v>303208.52800000005</v>
+      </c>
+      <c r="I45" s="32">
         <f t="shared" si="13"/>
         <v>353743.28266666667</v>
       </c>
-      <c r="D45" s="34">
-        <f t="shared" si="13"/>
-        <v>707486.56533333333</v>
-      </c>
-      <c r="E45" s="32">
-        <f t="shared" si="13"/>
-        <v>1061229.8480000002</v>
-      </c>
-      <c r="F45" s="34">
-        <f t="shared" si="13"/>
-        <v>1414973.1306666667</v>
-      </c>
-      <c r="G45" s="32">
-        <f t="shared" si="13"/>
-        <v>1768716.4133333333</v>
-      </c>
-      <c r="H45" s="34">
-        <f t="shared" si="13"/>
-        <v>2122459.6960000005</v>
-      </c>
-      <c r="I45" s="32">
-        <f t="shared" si="13"/>
-        <v>2476202.9786666669</v>
-      </c>
       <c r="J45" s="34">
         <f t="shared" si="13"/>
-        <v>2829946.2613333333</v>
+        <v>404278.03733333334</v>
       </c>
       <c r="K45" s="32">
         <f t="shared" si="13"/>
-        <v>3183689.5440000002</v>
+        <v>454812.79200000002</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -4584,44 +5742,43 @@
         <v>148</v>
       </c>
       <c r="B46" s="34">
-        <f t="shared" ref="B46:K46" si="14">B$43*ABS($G22-$H22)/9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C46" s="32">
+        <f t="shared" ref="B46:K46" si="14">C$43*ABS($G22-$H22)/9</f>
+        <v>58911.421333333332</v>
+      </c>
+      <c r="D46" s="34">
         <f t="shared" si="14"/>
         <v>117822.84266666666</v>
       </c>
-      <c r="D46" s="34">
+      <c r="E46" s="32">
+        <f t="shared" si="14"/>
+        <v>176734.26400000002</v>
+      </c>
+      <c r="F46" s="34">
         <f t="shared" si="14"/>
         <v>235645.68533333333</v>
       </c>
-      <c r="E46" s="32">
+      <c r="G46" s="32">
+        <f t="shared" si="14"/>
+        <v>294557.10666666669</v>
+      </c>
+      <c r="H46" s="34">
         <f t="shared" si="14"/>
         <v>353468.52800000005</v>
       </c>
-      <c r="F46" s="34">
+      <c r="I46" s="32">
+        <f t="shared" si="14"/>
+        <v>412379.94933333335</v>
+      </c>
+      <c r="J46" s="34">
         <f t="shared" si="14"/>
         <v>471291.37066666665</v>
       </c>
-      <c r="G46" s="32">
-        <f t="shared" si="14"/>
-        <v>589114.21333333338</v>
-      </c>
-      <c r="H46" s="34">
-        <f t="shared" si="14"/>
-        <v>706937.0560000001</v>
-      </c>
-      <c r="I46" s="32">
-        <f t="shared" si="14"/>
-        <v>824759.8986666667</v>
-      </c>
-      <c r="J46" s="34">
-        <f t="shared" si="14"/>
-        <v>942582.74133333331</v>
-      </c>
       <c r="K46" s="32">
         <f t="shared" si="14"/>
-        <v>1060405.584</v>
+        <v>530202.79200000002</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -4629,11 +5786,10 @@
         <v>159</v>
       </c>
       <c r="B47" s="34">
-        <f t="shared" ref="B47:K47" si="15">B$43*ABS($G23-$H23)/9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C47" s="32">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B47:K47" si="15">C$43*ABS($G23-$H23)/9</f>
         <v>33982.461333333333</v>
       </c>
       <c r="D47" s="34">
@@ -4674,44 +5830,43 @@
         <v>151</v>
       </c>
       <c r="B48" s="34">
-        <f t="shared" ref="B48:K48" si="16">B$43*ABS($G24-$H24)/9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C48" s="32">
-        <f t="shared" si="16"/>
-        <v>924207.68533333333</v>
+        <f t="shared" ref="B48:K48" si="16">C$43*ABS($G24-$H24)/9</f>
+        <v>66014.834666666662</v>
       </c>
       <c r="D48" s="34">
         <f t="shared" si="16"/>
-        <v>1848415.3706666667</v>
+        <v>132029.66933333332</v>
       </c>
       <c r="E48" s="32">
         <f t="shared" si="16"/>
-        <v>2772623.0559999999</v>
+        <v>198044.50399999999</v>
       </c>
       <c r="F48" s="34">
         <f t="shared" si="16"/>
-        <v>3696830.7413333333</v>
+        <v>264059.33866666665</v>
       </c>
       <c r="G48" s="32">
         <f t="shared" si="16"/>
-        <v>4621038.4266666658</v>
+        <v>330074.17333333334</v>
       </c>
       <c r="H48" s="34">
         <f t="shared" si="16"/>
-        <v>5545246.1119999997</v>
+        <v>396089.00799999997</v>
       </c>
       <c r="I48" s="32">
         <f t="shared" si="16"/>
-        <v>6469453.7973333336</v>
+        <v>462103.84266666666</v>
       </c>
       <c r="J48" s="34">
         <f t="shared" si="16"/>
-        <v>7393661.4826666666</v>
+        <v>528118.6773333333</v>
       </c>
       <c r="K48" s="32">
         <f t="shared" si="16"/>
-        <v>8317869.1679999996</v>
+        <v>594133.51199999999</v>
       </c>
     </row>
   </sheetData>
@@ -4726,7 +5881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -4856,308 +6011,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3645</v>
-      </c>
-      <c r="F2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="23">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="J2" s="19">
-        <f>$B$10+I2*(1-$B$10)</f>
-        <v>0.28505000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2817</v>
-      </c>
-      <c r="F3">
-        <v>894</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="H3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="23">
-        <v>0</v>
-      </c>
-      <c r="J3" s="19">
-        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3853</v>
-      </c>
-      <c r="F4">
-        <v>1280</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I4" s="23">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3411</v>
-      </c>
-      <c r="F5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="H5" t="s">
-        <v>158</v>
-      </c>
-      <c r="I5" s="23">
-        <v>8.8400000000000006E-2</v>
-      </c>
-      <c r="J5" s="19">
-        <f t="shared" si="0"/>
-        <v>0.27983599999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>1677</v>
-      </c>
-      <c r="F6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="H6" t="s">
-        <v>162</v>
-      </c>
-      <c r="I6" s="23">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="J6" s="19">
-        <f t="shared" si="0"/>
-        <v>0.28742000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2419</v>
-      </c>
-      <c r="F7">
-        <v>769</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="H7" t="s">
-        <v>167</v>
-      </c>
-      <c r="I7" s="23">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="J7" s="19">
-        <f t="shared" si="0"/>
-        <v>0.27169900000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3990</v>
-      </c>
-      <c r="F8" t="s">
-        <v>175</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" t="s">
-        <v>171</v>
-      </c>
-      <c r="I8" s="23">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="J8" s="19">
-        <f t="shared" si="0"/>
-        <v>0.24870999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="22">
-        <v>0.21</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="18"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add co2 cost/price calculations
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_FT_2023/data/HERON_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B3E8E-5E1C-4B43-9BA0-77827BC645D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D1045-6B7A-3B42-9822-F7089284E881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="7" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="10" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Sweep values" sheetId="10" r:id="rId8"/>
     <sheet name="Capacity_Market" sheetId="3" r:id="rId9"/>
     <sheet name="NPP_capacities" sheetId="12" r:id="rId10"/>
+    <sheet name="CO2 price EU" sheetId="16" r:id="rId11"/>
+    <sheet name="CO2 costs" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="244">
   <si>
     <t>Source</t>
   </si>
@@ -734,14 +736,58 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average exchange rate </t>
+  </si>
+  <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Average inflation 2020-2023</t>
+  </si>
+  <si>
+    <t>Conversion 2023 to 2020 USD</t>
+  </si>
+  <si>
+    <t>CO2 to H2 ratio</t>
+  </si>
+  <si>
+    <t>kg-CO2/kg-H2</t>
+  </si>
+  <si>
+    <t>CO2 prices 2019-2023 (Euro/ton)</t>
+  </si>
+  <si>
+    <t>Modelling USD(2020)/kg-H2</t>
+  </si>
+  <si>
+    <t>CO2 prices 2019-2023 (USD(2020)/kg)</t>
+  </si>
+  <si>
+    <t>Addtla cost $/ton-CO2</t>
+  </si>
+  <si>
+    <t>$/kg-H2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -796,7 +842,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,6 +857,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,7 +1032,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1018,12 +1070,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2455,10 +2511,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="37"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2890,12 +2946,183 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82E003A-465B-4F4D-AB31-9E82E29DDFB6}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2">
+        <v>16.11</v>
+      </c>
+      <c r="C2" s="35">
+        <v>43906</v>
+      </c>
+      <c r="E2">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="36">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="I2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3">
+        <v>104.81</v>
+      </c>
+      <c r="C3" s="35">
+        <v>44991</v>
+      </c>
+      <c r="E3">
+        <v>2023</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1.0861000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="39">
+        <f>B2*G2/1000</f>
+        <v>1.8397619999999996E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="39">
+        <f>B3*G3/(J2*1000)</f>
+        <v>9.6469611016949161E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="40">
+        <f>B6*Transfer_rates!$B$22</f>
+        <v>0.11399309647058822</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="40">
+        <f>B7*Transfer_rates!$B$22</f>
+        <v>0.59773327610501836</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF2C446-1B6D-5E44-9E7E-E1AC0C39F0C4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="39">
+        <f>A2*Transfer_rates!$B$22/1000</f>
+        <v>0.18588235294117647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="39">
+        <f>A3*Transfer_rates!$B$22/1000</f>
+        <v>0.37176470588235294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2930,26 +3157,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3021,15 +3248,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -3107,22 +3334,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -3136,11 +3363,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3161,6 +3388,18 @@
       </c>
       <c r="C20" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22">
+        <f>B7/B8</f>
+        <v>6.1960784313725492</v>
+      </c>
+      <c r="C22" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4679,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4835,28 +5074,28 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35" t="s">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35" t="s">
+      <c r="F18" s="37"/>
+      <c r="G18" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="H18" s="35"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
       <c r="C19" t="s">
         <v>98</v>
       </c>
@@ -5661,7 +5900,7 @@
         <v>66014.834666666662</v>
       </c>
       <c r="D44" s="34">
-        <f t="shared" ref="C44:J44" si="12">D$43*ABS($G20-$H20)/9</f>
+        <f t="shared" ref="D44:J44" si="12">D$43*ABS($G20-$H20)/9</f>
         <v>132029.66933333332</v>
       </c>
       <c r="E44" s="32">
@@ -5701,7 +5940,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="32">
-        <f t="shared" ref="B45:K45" si="13">C$43*ABS($G21-$H21)/9</f>
+        <f t="shared" ref="C45:K45" si="13">C$43*ABS($G21-$H21)/9</f>
         <v>50534.754666666668</v>
       </c>
       <c r="D45" s="34">
@@ -5745,7 +5984,7 @@
         <v>10</v>
       </c>
       <c r="C46" s="32">
-        <f t="shared" ref="B46:K46" si="14">C$43*ABS($G22-$H22)/9</f>
+        <f t="shared" ref="C46:K46" si="14">C$43*ABS($G22-$H22)/9</f>
         <v>58911.421333333332</v>
       </c>
       <c r="D46" s="34">
@@ -5789,7 +6028,7 @@
         <v>10</v>
       </c>
       <c r="C47" s="32">
-        <f t="shared" ref="B47:K47" si="15">C$43*ABS($G23-$H23)/9</f>
+        <f t="shared" ref="C47:K47" si="15">C$43*ABS($G23-$H23)/9</f>
         <v>33982.461333333333</v>
       </c>
       <c r="D47" s="34">
@@ -5833,7 +6072,7 @@
         <v>10</v>
       </c>
       <c r="C48" s="32">
-        <f t="shared" ref="B48:K48" si="16">C$43*ABS($G24-$H24)/9</f>
+        <f t="shared" ref="C48:K48" si="16">C$43*ABS($G24-$H24)/9</f>
         <v>66014.834666666662</v>
       </c>
       <c r="D48" s="34">

</xml_diff>